<commit_message>
Updated ITA_grids model - 2025-08-13 21:36
</commit_message>
<xml_diff>
--- a/VerveStacks_ITA_grids/SuppXLS/trades/scentrade__trade_links.xlsx
+++ b/VerveStacks_ITA_grids/SuppXLS/trades/scentrade__trade_links.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Veda\Veda\Veda_models\vervestacks_models\VerveStacks_ITA_grids\SuppXLS\trades\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F987885E-ED1E-414B-94DF-B0E8DD889474}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{47D5904C-AD16-46C8-91C4-823317CAA4DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{F94586EA-B355-4D39-86C8-E75443438ACF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="17475" xr2:uid="{59CC8620-3822-4E85-BB03-914695FADB5A}"/>
   </bookViews>
   <sheets>
     <sheet name="grid_links" sheetId="1" r:id="rId1"/>
@@ -4194,8 +4194,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
       <b/>
-      <sz val="8"/>
+      <sz val="9"/>
       <color rgb="FFFFFFFF"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -4211,12 +4217,6 @@
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color theme="1"/>
       <name val="Segoe UI"/>
       <family val="2"/>
     </font>
@@ -4291,13 +4291,13 @@
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4313,6 +4313,61 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>266700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C427A62C-E600-2794-C21A-4C917FBA0E18}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5245100" y="12700"/>
+          <a:ext cx="990600" cy="254000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4631,7 +4686,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0484DA91-EB46-47B7-A892-ECCB61F06590}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A4576B-6420-4680-B52F-C104DB7CA7DE}">
   <dimension ref="A1:L682"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -4646,7 +4701,7 @@
     <col min="12" max="12" width="30.59765625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="20" customHeight="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:12" ht="22.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>1202</v>
       </c>
@@ -4657,8 +4712,6 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
       <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
     </row>
     <row r="3" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="B3" s="2" t="s">
@@ -24361,8 +24414,9 @@
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>